<commit_message>
Add edit and delete
Automate the ability to edit and delete
</commit_message>
<xml_diff>
--- a/Project4_34202676/CMPG323 EcoPower Logistics Data.xlsx
+++ b/Project4_34202676/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashto\Desktop\Code\CMPG-323-Project4---34202676\Project4_34202676\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DA89BE-21E8-486A-9ADF-9E20AF7A4D83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00F7B8E-B67D-43F7-A509-06FC26D6BA06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -730,7 +730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -1713,7 +1713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>